<commit_message>
Moving wallet to its own Wallet contract
</commit_message>
<xml_diff>
--- a/VAR_main_functions.xlsx
+++ b/VAR_main_functions.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak\Dropbox\WORK\EthDev\ruby_VAR\xlsx-scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\AK\github_T460\Blue-Frontiers\varyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11794751-88B9-42F1-8D1B-1D61519B6EE0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E82B2CC-4C8A-4A93-A775-4B27A1BF9486}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="1" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Functions and Events" sheetId="1" r:id="rId1"/>
+    <sheet name="Changes to variables" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>mintTokens()</t>
   </si>
@@ -139,13 +140,127 @@
   </si>
   <si>
     <t>(the highlighted functions emit the events)</t>
+  </si>
+  <si>
+    <t>[m] refundClaimed</t>
+  </si>
+  <si>
+    <t>refund</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>totalEthContributed</t>
+  </si>
+  <si>
+    <t>[m] ethContributed</t>
+  </si>
+  <si>
+    <t>eth issued</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>...tokensMinted</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>...tokensIcoBonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ..tokensIcoOffline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ..tokensIcoCrowd</t>
+  </si>
+  <si>
+    <t>...tokensIcoIssued</t>
+  </si>
+  <si>
+    <t>tb</t>
+  </si>
+  <si>
+    <t>ERC20</t>
+  </si>
+  <si>
+    <t>tokensIssuedTotal</t>
+  </si>
+  <si>
+    <t>[m] balancesBonus</t>
+  </si>
+  <si>
+    <t>[m] balancesOffline</t>
+  </si>
+  <si>
+    <t>[m] balances</t>
+  </si>
+  <si>
+    <t>tokens issued</t>
+  </si>
+  <si>
+    <t>-er</t>
+  </si>
+  <si>
+    <t>totalEthPending</t>
+  </si>
+  <si>
+    <t>[m] ethPending</t>
+  </si>
+  <si>
+    <t>eth pending</t>
+  </si>
+  <si>
+    <t>-t</t>
+  </si>
+  <si>
+    <t>-tm</t>
+  </si>
+  <si>
+    <t>tokensIcoPending</t>
+  </si>
+  <si>
+    <t>[m] balancesPending</t>
+  </si>
+  <si>
+    <t>tokens pending</t>
+  </si>
+  <si>
+    <t>pBlacklist</t>
+  </si>
+  <si>
+    <t>processTokenIssue</t>
+  </si>
+  <si>
+    <t>processWhitelisting</t>
+  </si>
+  <si>
+    <t>buyTokensWhitelist</t>
+  </si>
+  <si>
+    <t>offlineTokensWhitelist</t>
+  </si>
+  <si>
+    <t>buyTokensPending</t>
+  </si>
+  <si>
+    <t>offlineTokensPending</t>
+  </si>
+  <si>
+    <t>mintTokensLocked</t>
+  </si>
+  <si>
+    <t>mintTokens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +284,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +305,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,16 +338,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA2E39F-B301-47FB-818E-31291739FEB1}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,4 +989,599 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF5875E-FA35-4A6F-A6CA-127874656F03}">
+  <dimension ref="A2:Y27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Y27" sqref="Y27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="3.7109375" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="12" max="13" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" customWidth="1"/>
+    <col min="15" max="16" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" customWidth="1"/>
+    <col min="18" max="19" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" customWidth="1"/>
+    <col min="22" max="22" width="2.85546875" customWidth="1"/>
+    <col min="23" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.85546875" customWidth="1"/>
+    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:25" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="E2" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="H3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="5"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="5"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="5"/>
+      <c r="U3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="Y3" s="2"/>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="H4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="5"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="5"/>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="U4" s="16">
+        <v>0</v>
+      </c>
+      <c r="W4" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="5"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="5"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="5"/>
+      <c r="U5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="Y5" s="2"/>
+    </row>
+    <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="H6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="5"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="5"/>
+      <c r="R6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="U6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="W6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y6" s="13"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="H7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="5"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="5"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="5"/>
+      <c r="U7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="H8" s="8"/>
+      <c r="J8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="5"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="5"/>
+      <c r="R8" s="6">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5"/>
+      <c r="U8" s="16">
+        <v>0</v>
+      </c>
+      <c r="W8" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="H9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="5"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="5"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="5"/>
+      <c r="U9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="Y9" s="2"/>
+    </row>
+    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="H10" s="8"/>
+      <c r="J10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="5"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="5"/>
+      <c r="R10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" s="5"/>
+      <c r="U10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="W10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y10" s="13"/>
+    </row>
+    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="H11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="5"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="5"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="5"/>
+      <c r="U11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="Y11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R12" s="7"/>
+      <c r="S12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="Y12" s="2"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="H13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="L13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="5"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="5"/>
+      <c r="U13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="H14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="7"/>
+      <c r="P14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="R14" s="7"/>
+      <c r="S14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="Y14" s="2"/>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="5"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="5"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="5"/>
+      <c r="U15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="Y15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="7"/>
+      <c r="P16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R16" s="7"/>
+      <c r="S16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="U16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="Y16" s="2"/>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="H17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" s="7"/>
+      <c r="P17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="R17" s="7"/>
+      <c r="S17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="Y17" s="2"/>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="H18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="5"/>
+      <c r="O18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18" s="5"/>
+      <c r="R18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S18" s="5"/>
+      <c r="U18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="H19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="L19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="5"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="5"/>
+      <c r="U19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="Y19" s="2"/>
+    </row>
+    <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="H20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O20" s="7"/>
+      <c r="P20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="R20" s="7"/>
+      <c r="S20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="5"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="5"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="5"/>
+      <c r="U21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="H22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="5"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="5"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="5"/>
+      <c r="U22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="Y22" s="2"/>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="H23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="5"/>
+      <c r="O23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P23" s="5"/>
+      <c r="R23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="S23" s="5"/>
+      <c r="U23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="Y23" s="2"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="H24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="5"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="5"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="5"/>
+      <c r="U24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="Y24" s="2"/>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="H25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="5"/>
+      <c r="O25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P25" s="5"/>
+      <c r="R25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="S25" s="5"/>
+      <c r="U25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="Y25" s="2"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y26" s="2"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y27" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code clean up, better offline contrinution acocunting
Some code cleanup, removed unnecessary comments.

Changed ico date variables to camel case (date_ico_presale, date_ico_main, date_ico_end, date_ico_deadline) to (dateIcoPresale, dateIcoMain, dateIcoEnd, dateIcoDeadline)

Added balancesPendingOffline mapping to help with accounting of offline contribution returns
</commit_message>
<xml_diff>
--- a/VAR_main_functions.xlsx
+++ b/VAR_main_functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\AK\github_T460\Blue-Frontiers\varyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E82B2CC-4C8A-4A93-A775-4B27A1BF9486}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C31618-722D-4660-AD5B-9719ACC9E598}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="1" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Functions and Events" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,100 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Alex Kampa</author>
+  </authors>
+  <commentList>
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{DB83F15E-7208-4B77-A2E9-E972CF95C131}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alex Kampa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+only when some offline tokens are being returned</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Alex Kampa</author>
+  </authors>
+  <commentList>
+    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{9CAA66AD-8B27-4C87-B704-7E0540C28731}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alex Kampa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+it may not be possible to issue all pending tokens</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R11" authorId="0" shapeId="0" xr:uid="{66027F4E-AD3E-4760-9E64-D9C0BB852AF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alex Kampa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+all or part of the ether may get returned</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
   <si>
     <t>mintTokens()</t>
   </si>
@@ -193,18 +285,12 @@
     <t>[m] balancesBonus</t>
   </si>
   <si>
-    <t>[m] balancesOffline</t>
-  </si>
-  <si>
     <t>[m] balances</t>
   </si>
   <si>
     <t>tokens issued</t>
   </si>
   <si>
-    <t>-er</t>
-  </si>
-  <si>
     <t>totalEthPending</t>
   </si>
   <si>
@@ -217,9 +303,6 @@
     <t>-t</t>
   </si>
   <si>
-    <t>-tm</t>
-  </si>
-  <si>
     <t>tokensIcoPending</t>
   </si>
   <si>
@@ -241,26 +324,53 @@
     <t>buyTokensWhitelist</t>
   </si>
   <si>
-    <t>offlineTokensWhitelist</t>
-  </si>
-  <si>
     <t>buyTokensPending</t>
   </si>
   <si>
-    <t>offlineTokensPending</t>
-  </si>
-  <si>
     <t>mintTokensLocked</t>
   </si>
   <si>
     <t>mintTokens</t>
+  </si>
+  <si>
+    <t>...[m] balancesPendingOffline</t>
+  </si>
+  <si>
+    <t>...[m] balancesOffline</t>
+  </si>
+  <si>
+    <t>-e</t>
+  </si>
+  <si>
+    <t>-tx</t>
+  </si>
+  <si>
+    <t>-ex</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>BuyOfflineWhitelist</t>
+  </si>
+  <si>
+    <t>buyOfflinePending</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>(OfflineTokenReturn)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,8 +401,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +452,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -357,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -372,23 +501,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,11 +840,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA2E39F-B301-47FB-818E-31291739FEB1}">
-  <dimension ref="A1:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA2E39F-B301-47FB-818E-31291739FEB1}">
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,6 +855,7 @@
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.42578125" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -876,7 +1014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -884,7 +1022,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -898,8 +1036,11 @@
       <c r="G18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -907,7 +1048,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>22</v>
@@ -923,7 +1064,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>24</v>
@@ -933,7 +1074,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>21</v>
@@ -943,7 +1084,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -951,7 +1092,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>27</v>
@@ -965,7 +1106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>28</v>
@@ -977,7 +1118,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -988,21 +1129,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF5875E-FA35-4A6F-A6CA-127874656F03}">
-  <dimension ref="A2:Y27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF5875E-FA35-4A6F-A6CA-127874656F03}">
+  <dimension ref="A2:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
     <col min="5" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="3.7109375" customWidth="1"/>
@@ -1014,55 +1156,61 @@
     <col min="18" max="19" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.85546875" customWidth="1"/>
     <col min="21" max="21" width="3.7109375" customWidth="1"/>
-    <col min="22" max="22" width="2.85546875" customWidth="1"/>
-    <col min="23" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.85546875" customWidth="1"/>
-    <col min="25" max="25" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.85546875" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="E2" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" s="18" t="s">
+    <row r="2" spans="1:24" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="E2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="R2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" s="17" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="20"/>
+      <c r="O2" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="P2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="20"/>
+      <c r="U2" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="W2" s="20"/>
+      <c r="X2" s="24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="H3" s="8"/>
@@ -1074,15 +1222,15 @@
       <c r="R3" s="7"/>
       <c r="S3" s="5"/>
       <c r="U3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="Y3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="16"/>
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1100,398 +1248,399 @@
         <v>0</v>
       </c>
       <c r="S4" s="5"/>
-      <c r="U4" s="16">
+      <c r="U4" s="2"/>
+      <c r="V4" s="17">
         <v>0</v>
       </c>
-      <c r="W4" s="16">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="H5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="15"/>
       <c r="L5" s="7"/>
       <c r="M5" s="5"/>
       <c r="O5" s="7"/>
       <c r="P5" s="5"/>
-      <c r="R5" s="7"/>
+      <c r="R5" s="6">
+        <v>0</v>
+      </c>
       <c r="S5" s="5"/>
       <c r="U5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="Y5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
+      <c r="V5" s="17">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="H6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="H6" s="8"/>
+      <c r="J6" s="8"/>
       <c r="L6" s="7"/>
       <c r="M6" s="5"/>
       <c r="O6" s="7"/>
       <c r="P6" s="5"/>
-      <c r="R6" s="15" t="s">
-        <v>63</v>
-      </c>
+      <c r="R6" s="7"/>
       <c r="S6" s="5"/>
-      <c r="U6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="W6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y6" s="13"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U6" s="2"/>
+      <c r="V6" s="16"/>
+      <c r="X6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="H7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="L7" s="7"/>
       <c r="M7" s="5"/>
       <c r="O7" s="7"/>
       <c r="P7" s="5"/>
-      <c r="R7" s="7"/>
+      <c r="R7" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="S7" s="5"/>
       <c r="U7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="Y7" s="2"/>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="V7" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="X7" s="13"/>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="H8" s="8"/>
-      <c r="J8" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="J8" s="8"/>
       <c r="L8" s="7"/>
       <c r="M8" s="5"/>
       <c r="O8" s="7"/>
       <c r="P8" s="5"/>
-      <c r="R8" s="6">
-        <v>0</v>
-      </c>
+      <c r="R8" s="7"/>
       <c r="S8" s="5"/>
-      <c r="U8" s="16">
-        <v>0</v>
-      </c>
-      <c r="W8" s="16">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U8" s="2"/>
+      <c r="V8" s="16"/>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="H9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="J9" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="L9" s="7"/>
       <c r="M9" s="5"/>
       <c r="O9" s="7"/>
       <c r="P9" s="5"/>
-      <c r="R9" s="7"/>
+      <c r="R9" s="6">
+        <v>0</v>
+      </c>
       <c r="S9" s="5"/>
       <c r="U9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="Y9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
+      <c r="V9" s="17">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2"/>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="H10" s="8"/>
-      <c r="J10" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="J10" s="8"/>
       <c r="L10" s="7"/>
       <c r="M10" s="5"/>
       <c r="O10" s="7"/>
       <c r="P10" s="5"/>
-      <c r="R10" s="15" t="s">
-        <v>58</v>
-      </c>
+      <c r="R10" s="7"/>
       <c r="S10" s="5"/>
-      <c r="U10" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="W10" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y10" s="13"/>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U10" s="2"/>
+      <c r="V10" s="16"/>
+      <c r="X10" s="2"/>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="H11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="J11" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="L11" s="7"/>
       <c r="M11" s="5"/>
       <c r="O11" s="7"/>
       <c r="P11" s="5"/>
-      <c r="R11" s="7"/>
+      <c r="R11" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="S11" s="5"/>
       <c r="U11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="Y11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="V11" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="X11" s="13"/>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
       <c r="H12" s="8"/>
       <c r="J12" s="8"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="M12" s="5"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="P12" s="5"/>
       <c r="R12" s="7"/>
-      <c r="S12" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="S12" s="5"/>
       <c r="U12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="Y12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V12" s="16"/>
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
       <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="H13" s="12" t="s">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>44</v>
       </c>
+      <c r="F13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="8"/>
       <c r="J13" s="8"/>
-      <c r="L13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M13" s="5"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="O13" s="7"/>
-      <c r="P13" s="5"/>
+      <c r="P13" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="R13" s="7"/>
-      <c r="S13" s="5"/>
+      <c r="S13" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="U13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="Y13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V13" s="16"/>
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="H14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="L14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M14" s="5"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="P14" s="5"/>
       <c r="R14" s="7"/>
-      <c r="S14" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="S14" s="5"/>
       <c r="U14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="Y14" s="2"/>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V14" s="16"/>
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="H15" s="8"/>
       <c r="J15" s="8"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="O15" s="7"/>
-      <c r="P15" s="5"/>
+      <c r="P15" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="R15" s="7"/>
-      <c r="S15" s="5"/>
+      <c r="S15" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="U15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="Y15" s="2"/>
-    </row>
-    <row r="16" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="V15" s="16"/>
+      <c r="X15" s="2"/>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
       <c r="H16" s="8"/>
       <c r="J16" s="8"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="M16" s="5"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="P16" s="5"/>
       <c r="R16" s="7"/>
-      <c r="S16" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="S16" s="5"/>
       <c r="U16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V16" s="16"/>
+      <c r="X16" s="2"/>
+    </row>
+    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H17" s="8"/>
       <c r="J17" s="8"/>
       <c r="L17" s="7"/>
       <c r="M17" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="O17" s="7"/>
       <c r="P17" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="U17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="Y17" s="2"/>
-    </row>
-    <row r="18" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V17" s="16"/>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="H18" s="8"/>
       <c r="J18" s="8"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="5"/>
-      <c r="O18" s="6" t="s">
+      <c r="M18" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="P18" s="5"/>
-      <c r="R18" s="6" t="s">
+      <c r="O18" s="7"/>
+      <c r="P18" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="S18" s="5"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="U18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="Y18" s="2"/>
-    </row>
-    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V18" s="16"/>
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="H19" s="8"/>
       <c r="J19" s="8"/>
-      <c r="L19" s="6" t="s">
+      <c r="L19" s="7"/>
+      <c r="M19" s="5"/>
+      <c r="O19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M19" s="5"/>
-      <c r="O19" s="7"/>
       <c r="P19" s="5"/>
-      <c r="R19" s="7"/>
+      <c r="R19" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="S19" s="5"/>
       <c r="U19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="Y19" s="2"/>
-    </row>
-    <row r="20" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V19" s="16"/>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="H20" s="8"/>
       <c r="J20" s="8"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="L20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" s="5"/>
       <c r="O20" s="7"/>
-      <c r="P20" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="R20" s="7"/>
-      <c r="S20" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="P20" s="5"/>
+      <c r="R20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S20" s="5"/>
       <c r="U20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V20" s="16"/>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
       <c r="H21" s="8"/>
       <c r="J21" s="8"/>
       <c r="L21" s="7"/>
-      <c r="M21" s="5"/>
+      <c r="M21" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="O21" s="7"/>
-      <c r="P21" s="5"/>
+      <c r="P21" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="R21" s="7"/>
-      <c r="S21" s="5"/>
+      <c r="S21" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="U21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="Y21" s="2"/>
-    </row>
-    <row r="22" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="V21" s="16"/>
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H22" s="8"/>
       <c r="J22" s="8"/>
       <c r="L22" s="7"/>
@@ -1501,87 +1650,108 @@
       <c r="R22" s="7"/>
       <c r="S22" s="5"/>
       <c r="U22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="Y22" s="2"/>
-    </row>
-    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
+      <c r="V22" s="16"/>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="H23" s="8"/>
       <c r="J23" s="8"/>
       <c r="L23" s="7"/>
       <c r="M23" s="5"/>
-      <c r="O23" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="O23" s="7"/>
       <c r="P23" s="5"/>
-      <c r="R23" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="R23" s="7"/>
       <c r="S23" s="5"/>
       <c r="U23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="Y23" s="2"/>
-    </row>
-    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="16"/>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="H24" s="8"/>
       <c r="J24" s="8"/>
       <c r="L24" s="7"/>
       <c r="M24" s="5"/>
-      <c r="O24" s="7"/>
+      <c r="O24" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="P24" s="5"/>
-      <c r="R24" s="7"/>
+      <c r="R24" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="S24" s="5"/>
       <c r="U24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="Y24" s="2"/>
-    </row>
-    <row r="25" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
+      <c r="V24" s="16"/>
+      <c r="X24" s="2"/>
+    </row>
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="H25" s="8"/>
       <c r="J25" s="8"/>
       <c r="L25" s="7"/>
       <c r="M25" s="5"/>
-      <c r="O25" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="O25" s="7"/>
       <c r="P25" s="5"/>
-      <c r="R25" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="R25" s="7"/>
       <c r="S25" s="5"/>
       <c r="U25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="Y25" s="2"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="Y26" s="2"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="V25" s="16"/>
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="H26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="5"/>
+      <c r="O26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P26" s="5"/>
+      <c r="R26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="S26" s="5"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="16"/>
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X27" s="2"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>38</v>
       </c>
-      <c r="Y27" s="2" t="b">
+      <c r="X28" s="2" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More code cleanup + adding balancesMinted
</commit_message>
<xml_diff>
--- a/VAR_main_functions.xlsx
+++ b/VAR_main_functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\AK\github_T460\Blue-Frontiers\varyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C31618-722D-4660-AD5B-9719ACC9E598}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FF6C05-B6C4-4FDA-A906-3F5960172F68}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="1" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Functions and Events" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>mintTokens()</t>
   </si>
@@ -351,9 +351,6 @@
     <t>Note:</t>
   </si>
   <si>
-    <t>BuyOfflineWhitelist</t>
-  </si>
-  <si>
     <t>buyOfflinePending</t>
   </si>
   <si>
@@ -364,6 +361,12 @@
   </si>
   <si>
     <t>(OfflineTokenReturn)</t>
+  </si>
+  <si>
+    <t>buyOfflineWhitelist</t>
+  </si>
+  <si>
+    <t>...[m] balancesMinted</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -503,6 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -843,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA2E39F-B301-47FB-818E-31291739FEB1}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -1037,7 +1041,7 @@
         <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1135,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF5875E-FA35-4A6F-A6CA-127874656F03}">
-  <dimension ref="A2:X30"/>
+  <dimension ref="A2:X31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,50 +1167,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" s="23" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="20"/>
-      <c r="O2" s="22" t="s">
+      <c r="N2" s="21"/>
+      <c r="O2" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="22" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="23" t="s">
+      <c r="S2" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="20"/>
-      <c r="U2" s="24" t="s">
+      <c r="T2" s="21"/>
+      <c r="U2" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="20"/>
-      <c r="X2" s="24" t="s">
+      <c r="W2" s="21"/>
+      <c r="X2" s="25" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1222,7 +1226,7 @@
       <c r="R3" s="7"/>
       <c r="S3" s="5"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="16"/>
+      <c r="V3" s="17"/>
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1249,7 +1253,7 @@
       </c>
       <c r="S4" s="5"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="17">
+      <c r="V4" s="18">
         <v>0</v>
       </c>
       <c r="X4" s="2"/>
@@ -1273,7 +1277,7 @@
       </c>
       <c r="S5" s="5"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="17">
+      <c r="V5" s="18">
         <v>0</v>
       </c>
       <c r="X5" s="2"/>
@@ -1290,7 +1294,7 @@
       <c r="R6" s="7"/>
       <c r="S6" s="5"/>
       <c r="U6" s="2"/>
-      <c r="V6" s="16"/>
+      <c r="V6" s="17"/>
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1314,7 +1318,7 @@
       </c>
       <c r="S7" s="5"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="18" t="s">
+      <c r="V7" s="19" t="s">
         <v>60</v>
       </c>
       <c r="X7" s="13"/>
@@ -1331,7 +1335,7 @@
       <c r="R8" s="7"/>
       <c r="S8" s="5"/>
       <c r="U8" s="2"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="17"/>
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1356,7 +1360,7 @@
       </c>
       <c r="S9" s="5"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="17">
+      <c r="V9" s="18">
         <v>0</v>
       </c>
       <c r="X9" s="2"/>
@@ -1373,7 +1377,7 @@
       <c r="R10" s="7"/>
       <c r="S10" s="5"/>
       <c r="U10" s="2"/>
-      <c r="V10" s="16"/>
+      <c r="V10" s="17"/>
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1395,7 +1399,7 @@
       </c>
       <c r="S11" s="5"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="18" t="s">
+      <c r="V11" s="19" t="s">
         <v>73</v>
       </c>
       <c r="X11" s="13"/>
@@ -1412,7 +1416,7 @@
       <c r="R12" s="7"/>
       <c r="S12" s="5"/>
       <c r="U12" s="2"/>
-      <c r="V12" s="16"/>
+      <c r="V12" s="17"/>
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1446,7 +1450,7 @@
         <v>51</v>
       </c>
       <c r="U13" s="2"/>
-      <c r="V13" s="16"/>
+      <c r="V13" s="17"/>
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1466,196 +1470,203 @@
       <c r="R14" s="7"/>
       <c r="S14" s="5"/>
       <c r="U14" s="2"/>
-      <c r="V14" s="16"/>
+      <c r="V14" s="17"/>
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="B15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H15" s="8"/>
       <c r="J15" s="8"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="5"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="P15" s="5"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="S15" s="5"/>
       <c r="U15" s="2"/>
-      <c r="V15" s="16"/>
+      <c r="V15" s="17"/>
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="H16" s="8"/>
       <c r="J16" s="8"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="5"/>
+      <c r="M16" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="O16" s="7"/>
-      <c r="P16" s="5"/>
+      <c r="P16" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="R16" s="7"/>
-      <c r="S16" s="5"/>
+      <c r="S16" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="U16" s="2"/>
-      <c r="V16" s="16"/>
+      <c r="V16" s="17"/>
       <c r="X16" s="2"/>
     </row>
     <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
       <c r="H17" s="8"/>
       <c r="J17" s="8"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="M17" s="5"/>
       <c r="O17" s="7"/>
-      <c r="P17" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="P17" s="5"/>
       <c r="R17" s="7"/>
-      <c r="S17" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="S17" s="5"/>
       <c r="U17" s="2"/>
-      <c r="V17" s="16"/>
+      <c r="V17" s="17"/>
       <c r="X17" s="2"/>
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="J18" s="8"/>
       <c r="L18" s="7"/>
       <c r="M18" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="O18" s="7"/>
       <c r="P18" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="R18" s="7"/>
       <c r="S18" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="U18" s="2"/>
-      <c r="V18" s="16"/>
+      <c r="V18" s="17"/>
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="H19" s="8"/>
       <c r="J19" s="8"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="5"/>
-      <c r="O19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P19" s="5"/>
-      <c r="R19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="S19" s="5"/>
+      <c r="M19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" s="7"/>
+      <c r="P19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="R19" s="7"/>
+      <c r="S19" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="U19" s="2"/>
-      <c r="V19" s="16"/>
+      <c r="V19" s="17"/>
       <c r="X19" s="2"/>
     </row>
     <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="H20" s="8"/>
       <c r="J20" s="8"/>
-      <c r="L20" s="6" t="s">
-        <v>44</v>
-      </c>
+      <c r="L20" s="7"/>
       <c r="M20" s="5"/>
-      <c r="O20" s="7"/>
+      <c r="O20" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="P20" s="5"/>
       <c r="R20" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S20" s="5"/>
       <c r="U20" s="2"/>
-      <c r="V20" s="16"/>
+      <c r="V20" s="17"/>
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="H21" s="8"/>
       <c r="J21" s="8"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="L21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" s="5"/>
       <c r="O21" s="7"/>
-      <c r="P21" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="R21" s="7"/>
-      <c r="S21" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="P21" s="5"/>
+      <c r="R21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="S21" s="5"/>
       <c r="U21" s="2"/>
-      <c r="V21" s="16"/>
+      <c r="V21" s="17"/>
       <c r="X21" s="2"/>
     </row>
     <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
       <c r="H22" s="8"/>
       <c r="J22" s="8"/>
       <c r="L22" s="7"/>
-      <c r="M22" s="5"/>
+      <c r="M22" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="O22" s="7"/>
-      <c r="P22" s="5"/>
+      <c r="P22" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="R22" s="7"/>
-      <c r="S22" s="5"/>
+      <c r="S22" s="11" t="s">
+        <v>46</v>
+      </c>
       <c r="U22" s="2"/>
-      <c r="V22" s="16"/>
+      <c r="V22" s="17"/>
       <c r="X22" s="2"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H23" s="8"/>
       <c r="J23" s="8"/>
       <c r="L23" s="7"/>
@@ -1665,87 +1676,102 @@
       <c r="R23" s="7"/>
       <c r="S23" s="5"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="16"/>
+      <c r="V23" s="17"/>
       <c r="X23" s="2"/>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="H24" s="8"/>
       <c r="J24" s="8"/>
       <c r="L24" s="7"/>
       <c r="M24" s="5"/>
-      <c r="O24" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="O24" s="7"/>
       <c r="P24" s="5"/>
-      <c r="R24" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="R24" s="7"/>
       <c r="S24" s="5"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="16"/>
+      <c r="V24" s="17"/>
       <c r="X24" s="2"/>
     </row>
     <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="H25" s="8"/>
       <c r="J25" s="8"/>
       <c r="L25" s="7"/>
       <c r="M25" s="5"/>
-      <c r="O25" s="7"/>
+      <c r="O25" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="P25" s="5"/>
-      <c r="R25" s="7"/>
+      <c r="R25" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="S25" s="5"/>
       <c r="U25" s="2"/>
-      <c r="V25" s="16"/>
+      <c r="V25" s="17"/>
       <c r="X25" s="2"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="H26" s="8"/>
       <c r="J26" s="8"/>
       <c r="L26" s="7"/>
       <c r="M26" s="5"/>
-      <c r="O26" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="O26" s="7"/>
       <c r="P26" s="5"/>
-      <c r="R26" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="R26" s="7"/>
       <c r="S26" s="5"/>
       <c r="U26" s="2"/>
-      <c r="V26" s="16"/>
+      <c r="V26" s="17"/>
       <c r="X26" s="2"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="H27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="5"/>
+      <c r="O27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P27" s="5"/>
+      <c r="R27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="S27" s="5"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="17"/>
       <c r="X27" s="2"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="X28" s="2"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>38</v>
       </c>
-      <c r="X28" s="2" t="b">
+      <c r="X29" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
18 decimals / formatting / checkDateOrder
+ token decimals changed to 18

+ formatting change to 4-space indents

+ added checkDateOrder() in VaryonIcoDates to simplify code

+ in processTokenIssue(), token adjustment made more compact
</commit_message>
<xml_diff>
--- a/VAR_main_functions.xlsx
+++ b/VAR_main_functions.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\AK\github_T460\Blue-Frontiers\varyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FF6C05-B6C4-4FDA-A906-3F5960172F68}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340E6C41-489B-4A06-8CBD-2FE267D10AE2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="1" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Functions and Events" sheetId="1" r:id="rId1"/>
     <sheet name="Changes to variables" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>mintTokens()</t>
   </si>
@@ -282,9 +283,6 @@
     <t>tokensIssuedTotal</t>
   </si>
   <si>
-    <t>[m] balancesBonus</t>
-  </si>
-  <si>
     <t>[m] balances</t>
   </si>
   <si>
@@ -367,6 +365,15 @@
   </si>
   <si>
     <t>...[m] balancesMinted</t>
+  </si>
+  <si>
+    <t>...[m] balancesBonus</t>
+  </si>
+  <si>
+    <t>addToWhitelist()</t>
+  </si>
+  <si>
+    <t>addToWhitelistParams()</t>
   </si>
 </sst>
 </file>
@@ -845,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA2E39F-B301-47FB-818E-31291739FEB1}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1034,9 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1041,12 +1050,14 @@
         <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1054,34 +1065,32 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1090,7 +1099,9 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1098,37 +1109,45 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1142,7 +1161,7 @@
   <dimension ref="A2:X31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,43 +1187,43 @@
   <sheetData>
     <row r="2" spans="1:24" ht="78.75" x14ac:dyDescent="0.25">
       <c r="E2" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I2" s="21"/>
       <c r="J2" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K2" s="21"/>
       <c r="L2" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N2" s="21"/>
       <c r="O2" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P2" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q2" s="21"/>
       <c r="R2" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S2" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T2" s="21"/>
       <c r="U2" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V2" s="26" t="s">
         <v>20</v>
@@ -1231,10 +1250,10 @@
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1260,7 +1279,7 @@
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -1299,7 +1318,7 @@
     </row>
     <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1314,12 +1333,12 @@
       <c r="O7" s="7"/>
       <c r="P7" s="5"/>
       <c r="R7" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S7" s="5"/>
       <c r="U7" s="2"/>
       <c r="V7" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X7" s="13"/>
     </row>
@@ -1340,10 +1359,10 @@
     </row>
     <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -1382,7 +1401,7 @@
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -1395,12 +1414,12 @@
       <c r="O11" s="7"/>
       <c r="P11" s="5"/>
       <c r="R11" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S11" s="5"/>
       <c r="U11" s="2"/>
       <c r="V11" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X11" s="13"/>
     </row>
@@ -1421,10 +1440,10 @@
     </row>
     <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
         <v>52</v>
@@ -1455,7 +1474,7 @@
     </row>
     <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -1475,7 +1494,7 @@
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>44</v>
@@ -1497,7 +1516,7 @@
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -1604,7 +1623,7 @@
       </c>
       <c r="P20" s="5"/>
       <c r="R20" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S20" s="5"/>
       <c r="U20" s="2"/>
@@ -1626,7 +1645,7 @@
       <c r="O21" s="7"/>
       <c r="P21" s="5"/>
       <c r="R21" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S21" s="5"/>
       <c r="U21" s="2"/>
@@ -1772,7 +1791,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1780,4 +1799,16 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A56751-4382-4374-B6D8-39E6B246F6A3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes + change to LockSlots
(not tested)
</commit_message>
<xml_diff>
--- a/VAR_main_functions.xlsx
+++ b/VAR_main_functions.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Dropbox\AK\github_T460\Blue-Frontiers\varyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340E6C41-489B-4A06-8CBD-2FE267D10AE2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684DDF2B-93FB-4879-839C-E879645FAD4F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" activeTab="1" xr2:uid="{F111E832-917D-40E5-8A40-F4671022BD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Functions and Events" sheetId="1" r:id="rId1"/>
     <sheet name="Changes to variables" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -1161,7 +1160,7 @@
   <dimension ref="A2:X31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,7 +1277,7 @@
       <c r="X4" s="2"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="9"/>
@@ -1493,7 +1492,7 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E15" s="10" t="s">
@@ -1799,16 +1798,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A56751-4382-4374-B6D8-39E6B246F6A3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>